<commit_message>
Create Client & Corrected Excels
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2482-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DELETE-VAR-INST-UPFRONT-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2482-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DELETE-VAR-INST-UPFRONT-Newcreateloan1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <t>principal1</t>
   </si>
   <si>
-    <t>2560-MS-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DATE-VAR-INST-UPFRONT</t>
+    <t>2480-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DATE-VAR-INST-UPFRONT</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -769,7 +769,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +892,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H3" sqref="H3:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>